<commit_message>
books link to book chapters
provided a list of books that need to be linked to book chapters in Wikidata
</commit_message>
<xml_diff>
--- a/divinity_law/doi_source_2022-02-11.xlsx
+++ b/divinity_law/doi_source_2022-02-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baskausj/github/vandycite/divinity_law/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\vandycite\divinity_law\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC18447-F40B-8046-B66D-71DEEDF467B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A53BD5B-F85C-4517-AC6C-9A7F1CFE3362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2160" windowWidth="37880" windowHeight="23260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doi_source_2022-02-11" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="686">
   <si>
     <t>qid</t>
   </si>
@@ -2072,13 +2072,25 @@
   </si>
   <si>
     <t>Cambridge</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2087,6 +2099,12 @@
     <font>
       <sz val="10"/>
       <color theme="8" tint="0.79998168889431442"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2141,7 +2159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2152,6 +2170,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2534,24 +2554,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I304"/>
+  <dimension ref="A1:J304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H52" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="63.6640625" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="125.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="9" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="63.6328125" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="56.08984375" customWidth="1"/>
+    <col min="6" max="6" width="0.6328125" customWidth="1"/>
+    <col min="7" max="7" width="22.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2573,8 +2594,17 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H1" t="s">
+        <v>682</v>
+      </c>
+      <c r="I1" t="s">
+        <v>683</v>
+      </c>
+      <c r="J1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2591,7 +2621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2610,8 +2640,11 @@
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2631,7 +2664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2651,7 +2684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2667,8 +2700,11 @@
       <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H6" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2687,8 +2723,11 @@
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H7" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2707,8 +2746,11 @@
       <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H8" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2727,8 +2769,11 @@
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2747,8 +2792,11 @@
       <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2767,8 +2815,11 @@
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H11" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -2787,8 +2838,11 @@
       <c r="G12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H12" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2808,7 +2862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2828,7 +2882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -2848,7 +2902,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -2868,7 +2922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -2888,7 +2942,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2908,7 +2962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -2928,7 +2982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -2948,7 +3002,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -2968,7 +3022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2985,7 +3039,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>63</v>
       </c>
@@ -3004,8 +3058,11 @@
       <c r="G23" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H23" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
@@ -3024,8 +3081,11 @@
       <c r="G24" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H24" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
@@ -3044,8 +3104,11 @@
       <c r="G25" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H25" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
@@ -3064,8 +3127,11 @@
       <c r="G26" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H26" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>63</v>
       </c>
@@ -3084,8 +3150,11 @@
       <c r="G27" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H27" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>63</v>
       </c>
@@ -3104,8 +3173,11 @@
       <c r="G28" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H28" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>63</v>
       </c>
@@ -3124,8 +3196,11 @@
       <c r="G29" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H29" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>63</v>
       </c>
@@ -3144,8 +3219,11 @@
       <c r="G30" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="H30" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>63</v>
       </c>
@@ -3171,7 +3249,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>63</v>
       </c>
@@ -3191,7 +3269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
@@ -3210,8 +3288,11 @@
       <c r="G33" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H33" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>63</v>
       </c>
@@ -3230,8 +3311,11 @@
       <c r="G34" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="H34" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>63</v>
       </c>
@@ -3251,7 +3335,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>63</v>
       </c>
@@ -3271,7 +3355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>63</v>
       </c>
@@ -3288,7 +3372,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -3308,7 +3392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>63</v>
       </c>
@@ -3328,7 +3412,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>63</v>
       </c>
@@ -3348,7 +3432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>117</v>
       </c>
@@ -3368,7 +3452,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>117</v>
       </c>
@@ -3384,8 +3468,11 @@
       <c r="G42" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H42" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>117</v>
       </c>
@@ -3401,8 +3488,11 @@
       <c r="G43" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H43" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>117</v>
       </c>
@@ -3418,8 +3508,11 @@
       <c r="G44" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H44" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>117</v>
       </c>
@@ -3435,8 +3528,11 @@
       <c r="G45" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H45" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>117</v>
       </c>
@@ -3452,8 +3548,11 @@
       <c r="G46" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H46" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>117</v>
       </c>
@@ -3469,8 +3568,11 @@
       <c r="G47" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H47" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>117</v>
       </c>
@@ -3486,8 +3588,11 @@
       <c r="G48" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H48" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>117</v>
       </c>
@@ -3503,8 +3608,11 @@
       <c r="G49" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H49" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>117</v>
       </c>
@@ -3520,8 +3628,11 @@
       <c r="G50" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H50" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>117</v>
       </c>
@@ -3541,7 +3652,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>117</v>
       </c>
@@ -3561,14 +3672,14 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="8" t="s">
         <v>148</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -3580,15 +3691,18 @@
       <c r="G53" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H53" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="8" t="s">
         <v>152</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -3600,8 +3714,11 @@
       <c r="G54" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H54" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>154</v>
       </c>
@@ -3621,7 +3738,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>159</v>
       </c>
@@ -3638,7 +3755,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>159</v>
       </c>
@@ -3658,7 +3775,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>159</v>
       </c>
@@ -3678,7 +3795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>159</v>
       </c>
@@ -3698,7 +3815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -3718,7 +3835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>159</v>
       </c>
@@ -3738,7 +3855,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>159</v>
       </c>
@@ -3758,7 +3875,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>159</v>
       </c>
@@ -3778,7 +3895,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>159</v>
       </c>
@@ -3798,7 +3915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>159</v>
       </c>
@@ -3815,7 +3932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>159</v>
       </c>
@@ -3835,7 +3952,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>159</v>
       </c>
@@ -3855,7 +3972,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>159</v>
       </c>
@@ -3875,7 +3992,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>159</v>
       </c>
@@ -3895,7 +4012,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>159</v>
       </c>
@@ -3915,7 +4032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>159</v>
       </c>
@@ -3935,7 +4052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>159</v>
       </c>
@@ -3955,7 +4072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>159</v>
       </c>
@@ -3975,7 +4092,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>159</v>
       </c>
@@ -3995,7 +4112,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>159</v>
       </c>
@@ -4015,7 +4132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>159</v>
       </c>
@@ -4035,7 +4152,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>159</v>
       </c>
@@ -4055,7 +4172,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>159</v>
       </c>
@@ -4075,7 +4192,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>159</v>
       </c>
@@ -4095,7 +4212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>159</v>
       </c>
@@ -4115,7 +4232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>159</v>
       </c>
@@ -4135,7 +4252,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>159</v>
       </c>
@@ -4155,7 +4272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>159</v>
       </c>
@@ -4175,7 +4292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>159</v>
       </c>
@@ -4195,7 +4312,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>159</v>
       </c>
@@ -4215,7 +4332,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>217</v>
       </c>
@@ -4234,8 +4351,11 @@
       <c r="G86" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H86" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>217</v>
       </c>
@@ -4255,7 +4375,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>217</v>
       </c>
@@ -4272,7 +4392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>217</v>
       </c>
@@ -4291,8 +4411,11 @@
       <c r="G89" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="90" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H89" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>217</v>
       </c>
@@ -4311,8 +4434,11 @@
       <c r="G90" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H90" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>217</v>
       </c>
@@ -4331,8 +4457,11 @@
       <c r="G91" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H91" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>217</v>
       </c>
@@ -4351,8 +4480,11 @@
       <c r="G92" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H92" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>217</v>
       </c>
@@ -4371,8 +4503,11 @@
       <c r="G93" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="94" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H93" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>217</v>
       </c>
@@ -4391,8 +4526,11 @@
       <c r="G94" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H94" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>217</v>
       </c>
@@ -4411,8 +4549,11 @@
       <c r="G95" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H95" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>217</v>
       </c>
@@ -4431,8 +4572,11 @@
       <c r="G96" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H96" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>217</v>
       </c>
@@ -4451,8 +4595,11 @@
       <c r="G97" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H97" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>217</v>
       </c>
@@ -4471,8 +4618,11 @@
       <c r="G98" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H98" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
         <v>217</v>
       </c>
@@ -4491,8 +4641,11 @@
       <c r="G99" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H99" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>247</v>
       </c>
@@ -4509,7 +4662,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>247</v>
       </c>
@@ -4529,7 +4682,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>247</v>
       </c>
@@ -4549,7 +4702,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>247</v>
       </c>
@@ -4569,7 +4722,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>247</v>
       </c>
@@ -4589,7 +4742,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>247</v>
       </c>
@@ -4609,7 +4762,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>247</v>
       </c>
@@ -4629,7 +4782,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>247</v>
       </c>
@@ -4649,7 +4802,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>247</v>
       </c>
@@ -4669,7 +4822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>267</v>
       </c>
@@ -4692,7 +4845,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
         <v>247</v>
       </c>
@@ -4709,7 +4862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>247</v>
       </c>
@@ -4729,7 +4882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>247</v>
       </c>
@@ -4749,7 +4902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>247</v>
       </c>
@@ -4769,7 +4922,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>279</v>
       </c>
@@ -4789,7 +4942,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>279</v>
       </c>
@@ -4809,14 +4962,14 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>279</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="8" t="s">
         <v>286</v>
       </c>
       <c r="E116" s="2" t="s">
@@ -4828,8 +4981,11 @@
       <c r="G116" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="117" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H116" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>289</v>
       </c>
@@ -4846,7 +5002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
         <v>289</v>
       </c>
@@ -4865,8 +5021,11 @@
       <c r="G118" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="119" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H118" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
         <v>289</v>
       </c>
@@ -4885,8 +5044,11 @@
       <c r="G119" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="120" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H119" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
         <v>289</v>
       </c>
@@ -4905,8 +5067,11 @@
       <c r="G120" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="121" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H120" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
         <v>289</v>
       </c>
@@ -4925,8 +5090,11 @@
       <c r="G121" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="122" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H121" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
         <v>289</v>
       </c>
@@ -4945,8 +5113,11 @@
       <c r="G122" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="123" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H122" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
         <v>289</v>
       </c>
@@ -4965,8 +5136,11 @@
       <c r="G123" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="124" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H123" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>289</v>
       </c>
@@ -4985,8 +5159,11 @@
       <c r="G124" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H124" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>289</v>
       </c>
@@ -5006,7 +5183,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>310</v>
       </c>
@@ -5026,7 +5203,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>310</v>
       </c>
@@ -5043,7 +5220,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="128" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
         <v>317</v>
       </c>
@@ -5060,7 +5237,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>317</v>
       </c>
@@ -5080,7 +5257,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>317</v>
       </c>
@@ -5100,7 +5277,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>317</v>
       </c>
@@ -5120,7 +5297,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>317</v>
       </c>
@@ -5140,7 +5317,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>317</v>
       </c>
@@ -5160,7 +5337,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>317</v>
       </c>
@@ -5180,7 +5357,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>317</v>
       </c>
@@ -5200,7 +5377,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>317</v>
       </c>
@@ -5220,7 +5397,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>317</v>
       </c>
@@ -5240,7 +5417,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>317</v>
       </c>
@@ -5260,7 +5437,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>317</v>
       </c>
@@ -5280,7 +5457,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>317</v>
       </c>
@@ -5300,7 +5477,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="141" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>317</v>
       </c>
@@ -5317,7 +5494,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>317</v>
       </c>
@@ -5331,7 +5508,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>317</v>
       </c>
@@ -5345,7 +5522,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>317</v>
       </c>
@@ -5365,7 +5542,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>317</v>
       </c>
@@ -5385,7 +5562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>317</v>
       </c>
@@ -5405,7 +5582,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="147" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
         <v>362</v>
       </c>
@@ -5422,7 +5599,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>362</v>
       </c>
@@ -5442,7 +5619,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>362</v>
       </c>
@@ -5462,7 +5639,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>362</v>
       </c>
@@ -5482,7 +5659,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>362</v>
       </c>
@@ -5502,7 +5679,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>362</v>
       </c>
@@ -5522,7 +5699,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>362</v>
       </c>
@@ -5542,7 +5719,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>362</v>
       </c>
@@ -5562,7 +5739,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>362</v>
       </c>
@@ -5582,7 +5759,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="156" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="s">
         <v>362</v>
       </c>
@@ -5599,7 +5776,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="157" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
         <v>362</v>
       </c>
@@ -5618,8 +5795,11 @@
       <c r="G157" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="158" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H157" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
         <v>362</v>
       </c>
@@ -5638,8 +5818,11 @@
       <c r="G158" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="159" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H158" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B159" s="2" t="s">
         <v>362</v>
       </c>
@@ -5658,8 +5841,11 @@
       <c r="G159" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="160" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H159" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
         <v>362</v>
       </c>
@@ -5678,8 +5864,11 @@
       <c r="G160" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="161" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H160" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="161" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
         <v>362</v>
       </c>
@@ -5698,8 +5887,11 @@
       <c r="G161" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="162" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H161" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="162" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
         <v>362</v>
       </c>
@@ -5718,8 +5910,11 @@
       <c r="G162" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="163" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H162" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
         <v>362</v>
       </c>
@@ -5738,8 +5933,11 @@
       <c r="G163" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="164" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H163" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="164" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B164" s="4" t="s">
         <v>362</v>
       </c>
@@ -5758,8 +5956,11 @@
       <c r="G164" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H164" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>362</v>
       </c>
@@ -5779,7 +5980,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>362</v>
       </c>
@@ -5799,7 +6000,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>362</v>
       </c>
@@ -5810,7 +6011,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>362</v>
       </c>
@@ -5830,7 +6031,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>362</v>
       </c>
@@ -5850,7 +6051,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="170" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>411</v>
       </c>
@@ -5867,7 +6068,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>411</v>
       </c>
@@ -5887,7 +6088,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>411</v>
       </c>
@@ -5907,7 +6108,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>411</v>
       </c>
@@ -5927,7 +6128,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>411</v>
       </c>
@@ -5947,7 +6148,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>411</v>
       </c>
@@ -5967,7 +6168,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="176" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>411</v>
       </c>
@@ -5987,7 +6188,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>411</v>
       </c>
@@ -6007,7 +6208,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="178" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>411</v>
       </c>
@@ -6027,7 +6228,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" s="1" t="s">
         <v>430</v>
       </c>
@@ -6044,7 +6245,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>430</v>
       </c>
@@ -6064,7 +6265,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>430</v>
       </c>
@@ -6084,7 +6285,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>430</v>
       </c>
@@ -6104,7 +6305,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>430</v>
       </c>
@@ -6124,7 +6325,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>430</v>
       </c>
@@ -6144,7 +6345,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="185" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>430</v>
       </c>
@@ -6164,7 +6365,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>430</v>
       </c>
@@ -6184,7 +6385,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="187" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B187" s="1" t="s">
         <v>430</v>
       </c>
@@ -6204,14 +6405,14 @@
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B188" s="2" t="s">
         <v>430</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="D188" s="2" t="s">
+      <c r="D188" s="8" t="s">
         <v>451</v>
       </c>
       <c r="E188" s="2" t="s">
@@ -6223,8 +6424,11 @@
       <c r="G188" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H188" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>430</v>
       </c>
@@ -6244,7 +6448,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>430</v>
       </c>
@@ -6264,7 +6468,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>430</v>
       </c>
@@ -6284,7 +6488,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>464</v>
       </c>
@@ -6304,7 +6508,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="193" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B193" s="1" t="s">
         <v>469</v>
       </c>
@@ -6321,7 +6525,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>469</v>
       </c>
@@ -6341,7 +6545,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="195" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B195" s="1" t="s">
         <v>469</v>
       </c>
@@ -6358,7 +6562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>469</v>
       </c>
@@ -6378,7 +6582,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>469</v>
       </c>
@@ -6398,11 +6602,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="198" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B198" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D198" s="2" t="s">
+      <c r="D198" s="8" t="s">
         <v>479</v>
       </c>
       <c r="E198" s="2" t="s">
@@ -6414,8 +6618,11 @@
       <c r="G198" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="I198" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="199" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>469</v>
       </c>
@@ -6435,7 +6642,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>469</v>
       </c>
@@ -6455,7 +6662,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="201" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
         <v>469</v>
       </c>
@@ -6472,7 +6679,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>469</v>
       </c>
@@ -6492,7 +6699,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>469</v>
       </c>
@@ -6512,7 +6719,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>469</v>
       </c>
@@ -6532,7 +6739,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>469</v>
       </c>
@@ -6552,7 +6759,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>469</v>
       </c>
@@ -6572,7 +6779,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>469</v>
       </c>
@@ -6592,7 +6799,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>469</v>
       </c>
@@ -6612,7 +6819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="209" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>469</v>
       </c>
@@ -6632,7 +6839,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="210" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="210" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B210" s="2" t="s">
         <v>469</v>
       </c>
@@ -6651,8 +6858,11 @@
       <c r="G210" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H210" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>469</v>
       </c>
@@ -6672,7 +6882,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="212" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="212" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B212" s="1" t="s">
         <v>469</v>
       </c>
@@ -6692,7 +6902,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>469</v>
       </c>
@@ -6712,7 +6922,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>469</v>
       </c>
@@ -6732,7 +6942,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>469</v>
       </c>
@@ -6752,7 +6962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B216" s="1" t="s">
         <v>529</v>
       </c>
@@ -6769,7 +6979,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>529</v>
       </c>
@@ -6789,7 +6999,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>529</v>
       </c>
@@ -6809,7 +7019,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="219" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B219" s="1" t="s">
         <v>529</v>
       </c>
@@ -6826,7 +7036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="220" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>529</v>
       </c>
@@ -6846,7 +7056,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="221" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>529</v>
       </c>
@@ -6866,7 +7076,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="222" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="222" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B222" s="1" t="s">
         <v>529</v>
       </c>
@@ -6883,7 +7093,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="223" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>529</v>
       </c>
@@ -6903,7 +7113,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="224" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="224" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>529</v>
       </c>
@@ -6923,7 +7133,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="225" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>529</v>
       </c>
@@ -6943,7 +7153,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="226" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>529</v>
       </c>
@@ -6963,7 +7173,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="227" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="227" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>529</v>
       </c>
@@ -6983,7 +7193,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="228" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>529</v>
       </c>
@@ -7003,7 +7213,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="229" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="229" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>529</v>
       </c>
@@ -7023,7 +7233,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="230" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="230" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>562</v>
       </c>
@@ -7043,7 +7253,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="231" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="231" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>562</v>
       </c>
@@ -7063,7 +7273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="232" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="232" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B232" s="2" t="s">
         <v>562</v>
       </c>
@@ -7082,15 +7292,18 @@
       <c r="G232" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="233" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H232" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="233" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B233" s="2" t="s">
         <v>562</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="D233" s="2" t="s">
+      <c r="D233" s="8" t="s">
         <v>573</v>
       </c>
       <c r="E233" s="2" t="s">
@@ -7102,8 +7315,11 @@
       <c r="G233" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H233" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="234" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>562</v>
       </c>
@@ -7123,7 +7339,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="235" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>562</v>
       </c>
@@ -7143,7 +7359,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="236" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="236" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B236" s="2" t="s">
         <v>562</v>
       </c>
@@ -7159,8 +7375,11 @@
       <c r="G236" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="237" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H236" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="237" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B237" s="2" t="s">
         <v>562</v>
       </c>
@@ -7179,8 +7398,11 @@
       <c r="G237" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="238" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H237" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="238" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B238" s="2" t="s">
         <v>562</v>
       </c>
@@ -7199,8 +7421,11 @@
       <c r="G238" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="239" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H238" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="239" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B239" s="2" t="s">
         <v>562</v>
       </c>
@@ -7219,8 +7444,11 @@
       <c r="G239" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="240" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H239" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="240" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B240" s="2" t="s">
         <v>562</v>
       </c>
@@ -7239,8 +7467,11 @@
       <c r="G240" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="241" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H240" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="241" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B241" s="2" t="s">
         <v>562</v>
       </c>
@@ -7259,8 +7490,11 @@
       <c r="G241" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="242" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H241" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="242" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B242" s="2" t="s">
         <v>562</v>
       </c>
@@ -7279,8 +7513,11 @@
       <c r="G242" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="243" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H242" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="243" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B243" s="2" t="s">
         <v>562</v>
       </c>
@@ -7299,8 +7536,11 @@
       <c r="G243" s="2" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H243" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>562</v>
       </c>
@@ -7320,7 +7560,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="245" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="245" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B245" s="1" t="s">
         <v>601</v>
       </c>
@@ -7337,7 +7577,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>601</v>
       </c>
@@ -7357,7 +7597,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>601</v>
       </c>
@@ -7377,7 +7617,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>601</v>
       </c>
@@ -7397,7 +7637,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>601</v>
       </c>
@@ -7417,7 +7657,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>601</v>
       </c>
@@ -7437,7 +7677,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>601</v>
       </c>
@@ -7457,7 +7697,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>601</v>
       </c>
@@ -7477,7 +7717,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>601</v>
       </c>
@@ -7497,7 +7737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
         <v>601</v>
       </c>
@@ -7517,7 +7757,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
         <v>601</v>
       </c>
@@ -7537,7 +7777,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="256" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="256" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B256" s="2" t="s">
         <v>601</v>
       </c>
@@ -7556,8 +7796,11 @@
       <c r="G256" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="257" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="H256" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="257" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
         <v>601</v>
       </c>
@@ -7577,11 +7820,11 @@
         <v>630</v>
       </c>
     </row>
-    <row r="258" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="258" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B258" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="D258" s="1" t="s">
+      <c r="D258" s="9" t="s">
         <v>632</v>
       </c>
       <c r="E258" s="1" t="s">
@@ -7594,7 +7837,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="259" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="259" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B259" s="2" t="s">
         <v>631</v>
       </c>
@@ -7613,8 +7856,11 @@
       <c r="G259" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="260" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H259" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="260" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B260" s="2" t="s">
         <v>631</v>
       </c>
@@ -7633,8 +7879,11 @@
       <c r="G260" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="261" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H260" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="261" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B261" s="2" t="s">
         <v>631</v>
       </c>
@@ -7653,8 +7902,11 @@
       <c r="G261" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="262" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H261" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="262" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B262" s="2" t="s">
         <v>631</v>
       </c>
@@ -7673,8 +7925,11 @@
       <c r="G262" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="263" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H262" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="263" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B263" s="2" t="s">
         <v>631</v>
       </c>
@@ -7693,8 +7948,11 @@
       <c r="G263" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="264" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H263" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="264" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B264" s="2" t="s">
         <v>631</v>
       </c>
@@ -7713,8 +7971,11 @@
       <c r="G264" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="265" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H264" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="265" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B265" s="2" t="s">
         <v>631</v>
       </c>
@@ -7733,8 +7994,11 @@
       <c r="G265" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="266" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H265" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="266" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B266" s="1" t="s">
         <v>648</v>
       </c>
@@ -7751,7 +8015,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="267" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="267" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
         <v>648</v>
       </c>
@@ -7771,7 +8035,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="268" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="268" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
         <v>648</v>
       </c>
@@ -7791,7 +8055,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="269" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
         <v>648</v>
       </c>
@@ -7811,7 +8075,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="270" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="270" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
         <v>648</v>
       </c>
@@ -7831,7 +8095,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="271" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="271" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
         <v>648</v>
       </c>
@@ -7851,7 +8115,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="272" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="272" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
         <v>648</v>
       </c>
@@ -7871,7 +8135,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
         <v>648</v>
       </c>
@@ -7891,7 +8155,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
         <v>648</v>
       </c>
@@ -7911,7 +8175,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
         <v>648</v>
       </c>
@@ -7931,7 +8195,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
         <v>648</v>
       </c>
@@ -7951,7 +8215,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
         <v>648</v>
       </c>
@@ -7971,7 +8235,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="278" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
         <v>7</v>
       </c>
@@ -7988,7 +8252,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="279" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B279" s="2" t="s">
         <v>7</v>
       </c>
@@ -8004,8 +8268,11 @@
       <c r="G279" s="2">
         <v>2016</v>
       </c>
-    </row>
-    <row r="280" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H279" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B280" s="5" t="s">
         <v>63</v>
       </c>
@@ -8022,7 +8289,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="281" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>676</v>
       </c>
@@ -8042,7 +8309,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="282" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B282" s="1" t="s">
         <v>159</v>
       </c>
@@ -8059,7 +8326,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="283" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B283" s="6" t="s">
         <v>217</v>
       </c>
@@ -8076,7 +8343,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="284" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B284" s="6" t="s">
         <v>247</v>
       </c>
@@ -8093,7 +8360,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="285" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B285" s="6" t="s">
         <v>289</v>
       </c>
@@ -8110,7 +8377,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="286" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B286" s="6" t="s">
         <v>317</v>
       </c>
@@ -8127,7 +8394,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="287" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B287" s="6" t="s">
         <v>317</v>
       </c>
@@ -8144,7 +8411,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="288" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B288" s="7" t="s">
         <v>362</v>
       </c>
@@ -8161,7 +8428,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="289" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="289" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B289" s="6" t="s">
         <v>362</v>
       </c>
@@ -8178,7 +8445,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="290" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="290" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B290" s="6" t="s">
         <v>362</v>
       </c>
@@ -8195,7 +8462,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="291" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="291" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B291" s="6" t="s">
         <v>411</v>
       </c>
@@ -8212,7 +8479,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="292" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="292" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B292" s="6" t="s">
         <v>430</v>
       </c>
@@ -8229,7 +8496,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="293" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="293" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B293" s="6" t="s">
         <v>469</v>
       </c>
@@ -8246,7 +8513,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="294" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="294" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B294" s="6" t="s">
         <v>469</v>
       </c>
@@ -8263,7 +8530,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="295" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="295" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B295" s="2" t="s">
         <v>469</v>
       </c>
@@ -8279,8 +8546,11 @@
       <c r="G295" s="2">
         <v>2007</v>
       </c>
-    </row>
-    <row r="296" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H295" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="296" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B296" s="1" t="s">
         <v>469</v>
       </c>
@@ -8297,7 +8567,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="297" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="297" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B297" s="6" t="s">
         <v>529</v>
       </c>
@@ -8314,7 +8584,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="298" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="298" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B298" s="6" t="s">
         <v>529</v>
       </c>
@@ -8331,7 +8601,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="299" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="299" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B299" s="6" t="s">
         <v>529</v>
       </c>
@@ -8348,7 +8618,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="300" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="300" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B300" s="6" t="s">
         <v>601</v>
       </c>
@@ -8365,7 +8635,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="301" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="301" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B301" s="6" t="s">
         <v>562</v>
       </c>
@@ -8382,7 +8652,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="302" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="302" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B302" s="6" t="s">
         <v>631</v>
       </c>
@@ -8399,7 +8669,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="303" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="303" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B303" s="6" t="s">
         <v>648</v>
       </c>
@@ -8416,7 +8686,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="304" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="304" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B304" s="6" t="s">
         <v>247</v>
       </c>

</xml_diff>